<commit_message>
redraw and fix % relevant table
</commit_message>
<xml_diff>
--- a/tables/tech_innov_totals.xlsx
+++ b/tables/tech_innov_totals.xlsx
@@ -18,12 +18,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
-    <t>PY</t>
+    <t>Technology</t>
   </si>
   <si>
     <t>RD</t>
+  </si>
+  <si>
+    <t>Demos</t>
   </si>
   <si>
     <t>Scaleup</t>
@@ -32,16 +35,19 @@
     <t>Demandpull</t>
   </si>
   <si>
+    <t>Nichemarkets</t>
+  </si>
+  <si>
     <t>Publicaccept</t>
   </si>
   <si>
-    <t>Demos</t>
+    <t>Total</t>
   </si>
   <si>
-    <t>Nichemarkets</t>
+    <t>distinct_Total</t>
   </si>
   <si>
-    <t>Technology</t>
+    <t>distinct_anyrating_Total</t>
   </si>
   <si>
     <t>distinct_alltech_Total</t>
@@ -75,15 +81,6 @@
   </si>
   <si>
     <t>Synonyms</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>distinct_Total</t>
-  </si>
-  <si>
-    <t>distinct_anyrating_Total</t>
   </si>
 </sst>
 </file>
@@ -432,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,104 +437,152 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="1">
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="n" s="1">
-        <v>1991</v>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="n" s="1">
-        <v>1992</v>
+        <v>7</v>
+      </c>
+      <c r="H2" t="n">
+        <v>247</v>
+      </c>
+      <c r="I2" t="n">
+        <v>186</v>
+      </c>
+      <c r="J2" t="n">
+        <v>260</v>
+      </c>
+      <c r="K2" t="n">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="n" s="1">
-        <v>1993</v>
+        <v>8</v>
+      </c>
+      <c r="H3" t="n">
+        <v>125</v>
+      </c>
+      <c r="I3" t="n">
+        <v>76</v>
+      </c>
+      <c r="J3" t="n">
+        <v>111</v>
+      </c>
+      <c r="K3" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="n" s="1">
-        <v>1994</v>
+        <v>5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>73</v>
+      </c>
+      <c r="I4" t="n">
+        <v>55</v>
+      </c>
+      <c r="J4" t="n">
+        <v>71</v>
+      </c>
+      <c r="K4" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -554,535 +599,290 @@
       <c r="G5" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="n" s="1">
-        <v>1995</v>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="n" s="1">
-        <v>1996</v>
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>101</v>
+      </c>
+      <c r="I6" t="n">
+        <v>80</v>
+      </c>
+      <c r="J6" t="n">
+        <v>117</v>
+      </c>
+      <c r="K6" t="n">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="n" s="1">
-        <v>1997</v>
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>26</v>
+      </c>
+      <c r="I7" t="n">
+        <v>18</v>
+      </c>
+      <c r="J7" t="n">
+        <v>31</v>
+      </c>
+      <c r="K7" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="n" s="1">
-        <v>1998</v>
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>13</v>
+      </c>
+      <c r="I8" t="n">
+        <v>9</v>
+      </c>
+      <c r="J8" t="n">
+        <v>10</v>
+      </c>
+      <c r="K8" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="n" s="1">
-        <v>1999</v>
+        <v>13</v>
+      </c>
+      <c r="H9" t="n">
+        <v>113</v>
+      </c>
+      <c r="I9" t="n">
+        <v>80</v>
+      </c>
+      <c r="J9" t="n">
+        <v>92</v>
+      </c>
+      <c r="K9" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="n" s="1">
-        <v>2000</v>
+        <v>22</v>
+      </c>
+      <c r="H10" t="n">
+        <v>233</v>
+      </c>
+      <c r="I10" t="n">
+        <v>189</v>
+      </c>
+      <c r="J10" t="n">
+        <v>357</v>
+      </c>
+      <c r="K10" t="n">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="n" s="1">
-        <v>2001</v>
+        <v>7</v>
+      </c>
+      <c r="H11" t="n">
+        <v>89</v>
+      </c>
+      <c r="I11" t="n">
+        <v>51</v>
+      </c>
+      <c r="J11" t="n">
+        <v>69</v>
+      </c>
+      <c r="K11" t="n">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>587</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>229</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="n" s="1">
-        <v>2002</v>
+        <v>71</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1021</v>
+      </c>
+      <c r="I12" t="n">
+        <v>745</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1127</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>545</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>284</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="n" s="1">
-        <v>2003</v>
-      </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="n" s="1">
-        <v>2004</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="n" s="1">
-        <v>2005</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="n" s="1">
-        <v>2006</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="n" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="n" s="1">
-        <v>2008</v>
-      </c>
-      <c r="B19" t="n">
-        <v>2</v>
-      </c>
-      <c r="C19" t="n">
-        <v>2</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="n" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B20" t="n">
-        <v>4</v>
-      </c>
-      <c r="C20" t="n">
-        <v>2</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="n" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="n" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B22" t="n">
-        <v>8</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="n" s="1">
-        <v>2012</v>
-      </c>
-      <c r="B23" t="n">
-        <v>11</v>
-      </c>
-      <c r="C23" t="n">
-        <v>4</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" t="n">
-        <v>2</v>
-      </c>
-      <c r="F23" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="n" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B24" t="n">
-        <v>10</v>
-      </c>
-      <c r="C24" t="n">
-        <v>6</v>
-      </c>
-      <c r="D24" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="n" s="1">
-        <v>2014</v>
-      </c>
-      <c r="B25" t="n">
-        <v>7</v>
-      </c>
-      <c r="C25" t="n">
-        <v>2</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="n" s="1">
-        <v>2015</v>
-      </c>
-      <c r="B26" t="n">
-        <v>7</v>
-      </c>
-      <c r="C26" t="n">
-        <v>2</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="n" s="1">
-        <v>2016</v>
-      </c>
-      <c r="B27" t="n">
-        <v>12</v>
-      </c>
-      <c r="C27" t="n">
-        <v>3</v>
-      </c>
-      <c r="D27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="n" s="1">
-        <v>2017</v>
-      </c>
-      <c r="B28" t="n">
-        <v>4</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="H13" t="s"/>
+      <c r="I13" t="s"/>
+      <c r="J13" t="s"/>
+      <c r="K13" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1104,34 +904,34 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s" s="1">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s" s="1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s" s="1">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s" s="1">
-        <v>8</v>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s" s="1">
-        <v>9</v>
+      <c r="A2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="n">
         <v>29.89473684210526</v>
@@ -1156,8 +956,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="s" s="1">
-        <v>10</v>
+      <c r="A3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B3" t="n">
         <v>25.84269662921348</v>
@@ -1182,8 +982,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s" s="1">
-        <v>11</v>
+      <c r="A4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B4" t="n">
         <v>54.02298850574713</v>
@@ -1208,8 +1008,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="s" s="1">
-        <v>12</v>
+      <c r="A5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B5" t="n">
         <v>50</v>
@@ -1234,8 +1034,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s" s="1">
-        <v>13</v>
+      <c r="A6" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B6" t="n">
         <v>29.86425339366516</v>
@@ -1260,8 +1060,8 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="s" s="1">
-        <v>14</v>
+      <c r="A7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B7" t="n">
         <v>36.36363636363637</v>
@@ -1286,8 +1086,8 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="s" s="1">
-        <v>15</v>
+      <c r="A8" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B8" t="n">
         <v>22.22222222222222</v>
@@ -1312,8 +1112,8 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" t="s" s="1">
-        <v>16</v>
+      <c r="A9" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B9" t="n">
         <v>36</v>
@@ -1338,8 +1138,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" t="s" s="1">
-        <v>17</v>
+      <c r="A10" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B10" t="n">
         <v>39.42307692307692</v>
@@ -1364,8 +1164,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" t="s" s="1">
-        <v>18</v>
+      <c r="A11" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B11" t="n">
         <v>13.8655462184874</v>
@@ -1390,8 +1190,8 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" t="s" s="1">
-        <v>19</v>
+      <c r="A12" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B12" t="n">
         <v>31.42398286937901</v>
@@ -1416,8 +1216,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" t="s" s="1">
-        <v>20</v>
+      <c r="A13" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B13" t="s"/>
       <c r="C13" t="s"/>
@@ -1438,7 +1238,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1447,115 +1247,115 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s" s="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s" s="1">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s" s="1">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s" s="1">
-        <v>21</v>
-      </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s" s="1">
-        <v>9</v>
+      <c r="A2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="n">
-        <v>54.61538461538461</v>
+        <v>100</v>
       </c>
       <c r="C2" t="n">
-        <v>3.461538461538462</v>
+        <v>69.23076923076923</v>
       </c>
       <c r="D2" t="n">
-        <v>24.23076923076923</v>
+        <v>78.75</v>
       </c>
       <c r="E2" t="n">
-        <v>9.615384615384617</v>
+        <v>58.13953488372093</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3846153846153846</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="G2" t="n">
-        <v>2.692307692307693</v>
+        <v>8.13953488372093</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>67.30245231607628</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="s" s="1">
-        <v>10</v>
+      <c r="A3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B3" t="n">
-        <v>41.44144144144144</v>
+        <v>100</v>
       </c>
       <c r="C3" t="n">
-        <v>6.306306306306306</v>
+        <v>41.17647058823529</v>
       </c>
       <c r="D3" t="n">
-        <v>30.63063063063063</v>
+        <v>64.15094339622641</v>
       </c>
       <c r="E3" t="n">
-        <v>24.32432432432433</v>
+        <v>54</v>
       </c>
       <c r="F3" t="n">
-        <v>2.702702702702703</v>
+        <v>100</v>
       </c>
       <c r="G3" t="n">
-        <v>7.207207207207207</v>
+        <v>20.51282051282051</v>
       </c>
       <c r="H3" t="n">
-        <v>100</v>
+        <v>60.09615384615385</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s" s="1">
-        <v>11</v>
+      <c r="A4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>66.19718309859155</v>
+        <v>100</v>
       </c>
       <c r="C4" t="n">
-        <v>1.408450704225352</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="D4" t="n">
-        <v>21.12676056338028</v>
+        <v>71.42857142857143</v>
       </c>
       <c r="E4" t="n">
-        <v>5.633802816901409</v>
+        <v>44.44444444444444</v>
       </c>
       <c r="F4" t="n">
-        <v>1.408450704225352</v>
+        <v>100</v>
       </c>
       <c r="G4" t="n">
-        <v>7.042253521126761</v>
+        <v>22.72727272727273</v>
       </c>
       <c r="H4" t="n">
-        <v>100</v>
+        <v>66.97247706422019</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="s" s="1">
-        <v>12</v>
+      <c r="A5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>11.11111111111111</v>
+        <v>100</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -1577,198 +1377,160 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s" s="1">
-        <v>13</v>
+      <c r="A6" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B6" t="n">
-        <v>56.41025641025641</v>
+        <v>100</v>
       </c>
       <c r="C6" t="n">
-        <v>4.273504273504273</v>
+        <v>22.72727272727273</v>
       </c>
       <c r="D6" t="n">
-        <v>20.51282051282051</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="E6" t="n">
-        <v>3.418803418803419</v>
+        <v>36.36363636363637</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1.70940170940171</v>
+        <v>11.76470588235294</v>
       </c>
       <c r="H6" t="n">
-        <v>100</v>
+        <v>66.01307189542483</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="s" s="1">
-        <v>14</v>
+      <c r="A7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B7" t="n">
-        <v>38.70967741935484</v>
+        <v>100</v>
       </c>
       <c r="C7" t="n">
-        <v>3.225806451612903</v>
+        <v>50</v>
       </c>
       <c r="D7" t="n">
-        <v>22.58064516129032</v>
+        <v>77.77777777777779</v>
       </c>
       <c r="E7" t="n">
-        <v>3.225806451612903</v>
+        <v>100</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>16.12903225806452</v>
+        <v>62.5</v>
       </c>
       <c r="H7" t="n">
-        <v>100</v>
+        <v>81.25</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="s" s="1">
-        <v>15</v>
+      <c r="A8" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" t="n">
+        <v>100</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>33.33333333333333</v>
+      </c>
+      <c r="H8" t="n">
+        <v>76.47058823529412</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="n">
+        <v>100</v>
+      </c>
+      <c r="C9" t="n">
+        <v>57.14285714285714</v>
+      </c>
+      <c r="D9" t="n">
+        <v>61.76470588235294</v>
+      </c>
+      <c r="E9" t="n">
+        <v>42.85714285714285</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>54.16666666666666</v>
+      </c>
+      <c r="H9" t="n">
+        <v>77.93103448275862</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="n">
+        <v>100</v>
+      </c>
+      <c r="C10" t="n">
+        <v>30.76923076923077</v>
+      </c>
+      <c r="D10" t="n">
+        <v>64.81481481481481</v>
+      </c>
+      <c r="E10" t="n">
         <v>50</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>15.71428571428571</v>
+      </c>
+      <c r="H10" t="n">
+        <v>59.74358974358974</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>20</v>
-      </c>
-      <c r="H8" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s" s="1">
-        <v>16</v>
-      </c>
-      <c r="B9" t="n">
-        <v>78.26086956521739</v>
-      </c>
-      <c r="C9" t="n">
-        <v>4.347826086956522</v>
-      </c>
-      <c r="D9" t="n">
-        <v>22.82608695652174</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3.260869565217391</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>14.1304347826087</v>
-      </c>
-      <c r="H9" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s" s="1">
-        <v>17</v>
-      </c>
-      <c r="B10" t="n">
-        <v>45.93837535014006</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1.120448179271709</v>
-      </c>
-      <c r="D10" t="n">
-        <v>9.803921568627452</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2.240896358543417</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>6.162464985994398</v>
-      </c>
-      <c r="H10" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s" s="1">
-        <v>18</v>
-      </c>
       <c r="B11" t="n">
-        <v>47.82608695652174</v>
+        <v>100</v>
       </c>
       <c r="C11" t="n">
-        <v>5.797101449275362</v>
+        <v>50</v>
       </c>
       <c r="D11" t="n">
-        <v>36.23188405797102</v>
+        <v>73.52941176470588</v>
       </c>
       <c r="E11" t="n">
-        <v>24.63768115942029</v>
+        <v>62.96296296296296</v>
       </c>
       <c r="F11" t="n">
-        <v>4.347826086956522</v>
+        <v>100</v>
       </c>
       <c r="G11" t="n">
-        <v>10.14492753623188</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="H11" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s" s="1">
-        <v>19</v>
-      </c>
-      <c r="B12" t="n">
-        <v>52.0851818988465</v>
-      </c>
-      <c r="C12" t="n">
-        <v>3.105590062111801</v>
-      </c>
-      <c r="D12" t="n">
-        <v>20.31943212067436</v>
-      </c>
-      <c r="E12" t="n">
-        <v>8.074534161490684</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.709849157054126</v>
-      </c>
-      <c r="G12" t="n">
-        <v>6.299911268855368</v>
-      </c>
-      <c r="H12" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s" s="1">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s"/>
-      <c r="C13" t="s"/>
-      <c r="D13" t="s"/>
-      <c r="E13" t="s"/>
-      <c r="F13" t="s"/>
-      <c r="G13" t="s"/>
-      <c r="H13" t="s"/>
+        <v>70.63492063492063</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1790,31 +1552,31 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s" s="1">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s" s="1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s" s="1">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s" s="1">
-        <v>9</v>
+      <c r="A2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="n">
         <v>100</v>
@@ -1836,8 +1598,8 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s" s="1">
-        <v>10</v>
+      <c r="A3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B3" t="n">
         <v>100</v>
@@ -1859,8 +1621,8 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s" s="1">
-        <v>11</v>
+      <c r="A4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B4" t="n">
         <v>100</v>
@@ -1882,8 +1644,8 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" t="s" s="1">
-        <v>12</v>
+      <c r="A5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B5" t="n">
         <v>100</v>
@@ -1905,8 +1667,8 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" t="s" s="1">
-        <v>13</v>
+      <c r="A6" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B6" t="n">
         <v>100</v>
@@ -1928,8 +1690,8 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s" s="1">
-        <v>14</v>
+      <c r="A7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B7" t="n">
         <v>100</v>
@@ -1951,8 +1713,8 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s" s="1">
-        <v>15</v>
+      <c r="A8" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B8" t="n">
         <v>100</v>
@@ -1974,8 +1736,8 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s" s="1">
-        <v>16</v>
+      <c r="A9" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B9" t="n">
         <v>100</v>
@@ -1997,8 +1759,8 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" t="s" s="1">
-        <v>17</v>
+      <c r="A10" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B10" t="n">
         <v>100</v>
@@ -2020,8 +1782,8 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" t="s" s="1">
-        <v>18</v>
+      <c r="A11" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B11" t="n">
         <v>100</v>
@@ -2043,8 +1805,8 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" t="s" s="1">
-        <v>19</v>
+      <c r="A12" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B12" t="n">
         <v>100</v>
@@ -2066,8 +1828,8 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" t="s" s="1">
-        <v>20</v>
+      <c r="A13" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B13" t="n">
         <v>100</v>
@@ -2108,37 +1870,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" t="s" s="1">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s" s="1">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s" s="1">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s" s="1">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s" s="1">
-        <v>19</v>
-      </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" t="n" s="1">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" t="n">
         <v>142</v>
@@ -2163,11 +1925,11 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" t="n" s="1">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="n">
         <v>46</v>
@@ -2192,11 +1954,11 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="n" s="1">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="n">
         <v>47</v>
@@ -2221,11 +1983,11 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" t="n" s="1">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -2250,11 +2012,11 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" t="n" s="1">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" t="n">
         <v>66</v>
@@ -2279,11 +2041,11 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" t="n" s="1">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
         <v>12</v>
@@ -2308,11 +2070,11 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" t="n" s="1">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8" t="n">
         <v>4</v>
@@ -2337,11 +2099,11 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" t="n" s="1">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" t="n">
         <v>72</v>
@@ -2366,11 +2128,11 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" t="n" s="1">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" t="n">
         <v>164</v>
@@ -2395,11 +2157,11 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" t="n" s="1">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" t="n">
         <v>33</v>

</xml_diff>